<commit_message>
Updated to add missing 2017 year data.
</commit_message>
<xml_diff>
--- a/InputData/indst/BSoAIGtAP/BAU Shr of Ag Indst Going to Anml Prdcts.xlsx
+++ b/InputData/indst/BSoAIGtAP/BAU Shr of Ag Indst Going to Anml Prdcts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\indst\BSoAIGtAP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Hong Kong\Models\eps-hongkong\InputData\indst\BSoAIGtAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -581,19 +581,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="68.73046875" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,102 +601,102 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -716,22 +716,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" customWidth="1"/>
-    <col min="2" max="2" width="25.3984375" customWidth="1"/>
-    <col min="3" max="3" width="26.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.265625" customWidth="1"/>
-    <col min="5" max="5" width="21.1328125" customWidth="1"/>
-    <col min="6" max="6" width="23.86328125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -739,7 +739,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -751,7 +751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -763,7 +763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -775,37 +775,37 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F13" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
         <v>29</v>
@@ -823,7 +823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -845,7 +845,7 @@
         <v>41512.799999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -867,7 +867,7 @@
         <v>527.88</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -889,7 +889,7 @@
         <v>706.26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -930,7 +930,7 @@
         <v>5088.16</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -954,7 +954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -979,7 +979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>1698.48</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>2768.6</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>1454.36</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>967.19999999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1088,32 +1088,32 @@
         <v>51587</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <f>SUMPRODUCT(D15:D26,F15:F26)/SUM(F15:F26)</f>
         <v>0.24377594409350131</v>
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D30" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <f>(B5/B3)+A29*(B4/B3)</f>
         <v>0.6232789702925996</v>
@@ -1129,140 +1129,143 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="8">
+      <c r="B1">
+        <v>2017</v>
+      </c>
+      <c r="C1" s="8">
         <v>2018</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2019</v>
       </c>
-      <c r="D1" s="8">
+      <c r="E1" s="8">
         <v>2020</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2021</v>
       </c>
-      <c r="F1" s="8">
+      <c r="G1" s="8">
         <v>2022</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>2023</v>
       </c>
-      <c r="H1" s="8">
+      <c r="I1" s="8">
         <v>2024</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>2025</v>
       </c>
-      <c r="J1" s="8">
+      <c r="K1" s="8">
         <v>2026</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>2027</v>
       </c>
-      <c r="L1" s="8">
+      <c r="M1" s="8">
         <v>2028</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>2029</v>
       </c>
-      <c r="N1" s="8">
+      <c r="O1" s="8">
         <v>2030</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>2031</v>
       </c>
-      <c r="P1" s="8">
+      <c r="Q1" s="8">
         <v>2032</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>2033</v>
       </c>
-      <c r="R1" s="8">
+      <c r="S1" s="8">
         <v>2034</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>2035</v>
       </c>
-      <c r="T1" s="8">
+      <c r="U1" s="8">
         <v>2036</v>
       </c>
-      <c r="U1">
+      <c r="V1">
         <v>2037</v>
       </c>
-      <c r="V1" s="8">
+      <c r="W1" s="8">
         <v>2038</v>
       </c>
-      <c r="W1">
+      <c r="X1">
         <v>2039</v>
       </c>
-      <c r="X1" s="8">
+      <c r="Y1" s="8">
         <v>2040</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <v>2041</v>
       </c>
-      <c r="Z1" s="8">
+      <c r="AA1" s="8">
         <v>2042</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <v>2043</v>
       </c>
-      <c r="AB1" s="8">
+      <c r="AC1" s="8">
         <v>2044</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <v>2045</v>
       </c>
-      <c r="AD1" s="8">
+      <c r="AE1" s="8">
         <v>2046</v>
       </c>
-      <c r="AE1">
+      <c r="AF1">
         <v>2047</v>
       </c>
-      <c r="AF1" s="8">
+      <c r="AG1" s="8">
         <v>2048</v>
       </c>
-      <c r="AG1">
+      <c r="AH1">
         <v>2049</v>
       </c>
-      <c r="AH1" s="8">
+      <c r="AI1" s="8">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2">
+        <f>$C2</f>
+        <v>0.6232789702925996</v>
+      </c>
+      <c r="C2" s="11">
         <f>Data!A33</f>
         <v>0.6232789702925996</v>
       </c>
-      <c r="C2">
-        <f>$B2</f>
-        <v>0.6232789702925996</v>
-      </c>
       <c r="D2">
-        <f t="shared" ref="D2:AH2" si="0">$B2</f>
+        <f>$C2</f>
         <v>0.6232789702925996</v>
       </c>
       <c r="E2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E2:AI2" si="0">$C2</f>
         <v>0.6232789702925996</v>
       </c>
       <c r="F2">
@@ -1378,6 +1381,10 @@
         <v>0.6232789702925996</v>
       </c>
       <c r="AH2">
+        <f t="shared" si="0"/>
+        <v>0.6232789702925996</v>
+      </c>
+      <c r="AI2">
         <f t="shared" si="0"/>
         <v>0.6232789702925996</v>
       </c>
@@ -1388,6 +1395,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1621,32 +1646,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20C1B51-73E0-4163-9C55-E18BB129F6D4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B6A4D5F-71D4-4C2E-878D-7A1DF124016B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884A611D-3614-4167-985A-C610892E85C0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884A611D-3614-4167-985A-C610892E85C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B6A4D5F-71D4-4C2E-878D-7A1DF124016B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20C1B51-73E0-4163-9C55-E18BB129F6D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>